<commit_message>
refactor: changed column names
</commit_message>
<xml_diff>
--- a/resources/sample-1.xlsx
+++ b/resources/sample-1.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t xml:space="preserve">id</t>
+    <t xml:space="preserve">number</t>
   </si>
   <si>
     <t xml:space="preserve">data</t>
@@ -206,11 +206,11 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9983" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>